<commit_message>
excel desconexion claro 100%
</commit_message>
<xml_diff>
--- a/reporte-Desconexion.xlsx
+++ b/reporte-Desconexion.xlsx
@@ -252,10 +252,10 @@
         <v>0</v>
       </c>
       <c r="E2" s="2">
-        <v>43346.9229282</v>
+        <v>43346.7979282</v>
       </c>
       <c r="F2" s="3">
-        <v>43346.9229282</v>
+        <v>43346.7979282</v>
       </c>
       <c r="O2" s="0" t="s">
         <v>24</v>
@@ -296,10 +296,10 @@
         <v>1234</v>
       </c>
       <c r="E3" s="2">
-        <v>43346.9285417</v>
+        <v>43346.8035417</v>
       </c>
       <c r="F3" s="3">
-        <v>43346.9285417</v>
+        <v>43346.8035417</v>
       </c>
       <c r="O3" s="0" t="s">
         <v>27</v>
@@ -340,10 +340,10 @@
         <v>1234</v>
       </c>
       <c r="E4" s="2">
-        <v>43352.9251042</v>
+        <v>43352.8001042</v>
       </c>
       <c r="F4" s="3">
-        <v>43352.9251042</v>
+        <v>43352.8001042</v>
       </c>
       <c r="O4" s="0" t="s">
         <v>24</v>
@@ -384,10 +384,10 @@
         <v>0</v>
       </c>
       <c r="E5" s="2">
-        <v>43357.8263773</v>
+        <v>43357.7013773</v>
       </c>
       <c r="F5" s="3">
-        <v>43357.8263773</v>
+        <v>43357.7013773</v>
       </c>
       <c r="O5" s="0" t="s">
         <v>25</v>
@@ -428,10 +428,10 @@
         <v>88888</v>
       </c>
       <c r="E6" s="2">
-        <v>43357.8372685</v>
+        <v>43357.7122685</v>
       </c>
       <c r="F6" s="3">
-        <v>43357.8372685</v>
+        <v>43357.7122685</v>
       </c>
       <c r="O6" s="0" t="s">
         <v>24</v>
@@ -472,10 +472,10 @@
         <v>88888</v>
       </c>
       <c r="E7" s="2">
-        <v>43357.8378819</v>
+        <v>43357.7128819</v>
       </c>
       <c r="F7" s="3">
-        <v>43357.8378819</v>
+        <v>43357.7128819</v>
       </c>
       <c r="O7" s="0" t="s">
         <v>24</v>
@@ -516,10 +516,10 @@
         <v>558</v>
       </c>
       <c r="E8" s="2">
-        <v>43357.839375</v>
+        <v>43357.714375</v>
       </c>
       <c r="F8" s="3">
-        <v>43357.839375</v>
+        <v>43357.714375</v>
       </c>
       <c r="O8" s="0" t="s">
         <v>24</v>
@@ -560,10 +560,10 @@
         <v>111111111</v>
       </c>
       <c r="E9" s="2">
-        <v>43357.8423264</v>
+        <v>43357.7173264</v>
       </c>
       <c r="F9" s="3">
-        <v>43357.8423264</v>
+        <v>43357.7173264</v>
       </c>
       <c r="O9" s="0" t="s">
         <v>24</v>
@@ -604,10 +604,10 @@
         <v>3333</v>
       </c>
       <c r="E10" s="2">
-        <v>43357.8451852</v>
+        <v>43357.7201852</v>
       </c>
       <c r="F10" s="3">
-        <v>43357.8451852</v>
+        <v>43357.7201852</v>
       </c>
       <c r="O10" s="0" t="s">
         <v>24</v>
@@ -648,10 +648,10 @@
         <v>141414</v>
       </c>
       <c r="E11" s="2">
-        <v>43357.8767593</v>
+        <v>43357.7517593</v>
       </c>
       <c r="F11" s="3">
-        <v>43357.8767593</v>
+        <v>43357.7517593</v>
       </c>
       <c r="O11" s="0" t="s">
         <v>24</v>
@@ -692,10 +692,10 @@
         <v>141414</v>
       </c>
       <c r="E12" s="2">
-        <v>43357.8771296</v>
+        <v>43357.7521296</v>
       </c>
       <c r="F12" s="3">
-        <v>43357.8771296</v>
+        <v>43357.7521296</v>
       </c>
       <c r="O12" s="0" t="s">
         <v>24</v>
@@ -736,10 +736,10 @@
         <v>141414</v>
       </c>
       <c r="E13" s="2">
-        <v>43357.8778472</v>
+        <v>43357.7528472</v>
       </c>
       <c r="F13" s="3">
-        <v>43357.8778472</v>
+        <v>43357.7528472</v>
       </c>
       <c r="O13" s="0" t="s">
         <v>24</v>
@@ -780,10 +780,10 @@
         <v>141414</v>
       </c>
       <c r="E14" s="2">
-        <v>43357.8787153</v>
+        <v>43357.7537153</v>
       </c>
       <c r="F14" s="3">
-        <v>43357.8787153</v>
+        <v>43357.7537153</v>
       </c>
       <c r="O14" s="0" t="s">
         <v>24</v>
@@ -824,10 +824,10 @@
         <v>8888</v>
       </c>
       <c r="E15" s="2">
-        <v>43362.7208681</v>
+        <v>43362.5958681</v>
       </c>
       <c r="F15" s="3">
-        <v>43362.7208681</v>
+        <v>43362.5958681</v>
       </c>
       <c r="O15" s="0" t="s">
         <v>24</v>
@@ -868,10 +868,10 @@
         <v>8888</v>
       </c>
       <c r="E16" s="2">
-        <v>43362.7210764</v>
+        <v>43362.5960764</v>
       </c>
       <c r="F16" s="3">
-        <v>43362.7210764</v>
+        <v>43362.5960764</v>
       </c>
       <c r="O16" s="0" t="s">
         <v>24</v>
@@ -912,10 +912,10 @@
         <v>13241324</v>
       </c>
       <c r="E17" s="2">
-        <v>43367.7739699</v>
+        <v>43367.6489699</v>
       </c>
       <c r="F17" s="3">
-        <v>43367.7739699</v>
+        <v>43367.6489699</v>
       </c>
       <c r="O17" s="0" t="s">
         <v>24</v>
@@ -956,10 +956,10 @@
         <v>2222222</v>
       </c>
       <c r="E18" s="2">
-        <v>43375.0155208</v>
+        <v>43374.8905208</v>
       </c>
       <c r="F18" s="3">
-        <v>43375.0155208</v>
+        <v>43374.8905208</v>
       </c>
       <c r="O18" s="0" t="s">
         <v>27</v>
@@ -1000,10 +1000,10 @@
         <v>666666</v>
       </c>
       <c r="E19" s="2">
-        <v>43375.5327894</v>
+        <v>43375.4077894</v>
       </c>
       <c r="F19" s="3">
-        <v>43375.5327894</v>
+        <v>43375.4077894</v>
       </c>
       <c r="O19" s="0" t="s">
         <v>24</v>
@@ -1044,10 +1044,10 @@
         <v>75577</v>
       </c>
       <c r="E20" s="2">
-        <v>43375.5418056</v>
+        <v>43375.4168056</v>
       </c>
       <c r="F20" s="3">
-        <v>43375.5418056</v>
+        <v>43375.4168056</v>
       </c>
       <c r="O20" s="0" t="s">
         <v>24</v>
@@ -1088,10 +1088,10 @@
         <v>8588</v>
       </c>
       <c r="E21" s="2">
-        <v>43376.1164699</v>
+        <v>43375.9914699</v>
       </c>
       <c r="F21" s="3">
-        <v>43376.1164699</v>
+        <v>43375.9914699</v>
       </c>
       <c r="O21" s="0" t="s">
         <v>24</v>
@@ -1132,10 +1132,10 @@
         <v>9999999999</v>
       </c>
       <c r="E22" s="2">
-        <v>43376.1265046</v>
+        <v>43376.0015046</v>
       </c>
       <c r="F22" s="3">
-        <v>43376.1265046</v>
+        <v>43376.0015046</v>
       </c>
       <c r="O22" s="0" t="s">
         <v>24</v>
@@ -1176,10 +1176,10 @@
         <v>3333</v>
       </c>
       <c r="E23" s="2">
-        <v>43376.6028588</v>
+        <v>43376.4778588</v>
       </c>
       <c r="F23" s="3">
-        <v>43376.6028588</v>
+        <v>43376.4778588</v>
       </c>
       <c r="O23" s="0" t="s">
         <v>24</v>
@@ -1220,10 +1220,10 @@
         <v>954628</v>
       </c>
       <c r="E24" s="2">
-        <v>43376.6285532</v>
+        <v>43376.5035532</v>
       </c>
       <c r="F24" s="3">
-        <v>43376.6285532</v>
+        <v>43376.5035532</v>
       </c>
       <c r="O24" s="0" t="s">
         <v>24</v>
@@ -1264,10 +1264,10 @@
         <v>6666</v>
       </c>
       <c r="E25" s="2">
-        <v>43376.6294444</v>
+        <v>43376.5044444</v>
       </c>
       <c r="F25" s="3">
-        <v>43376.6294444</v>
+        <v>43376.5044444</v>
       </c>
       <c r="O25" s="0" t="s">
         <v>24</v>
@@ -1308,10 +1308,10 @@
         <v>33333</v>
       </c>
       <c r="E26" s="2">
-        <v>43376.6320486</v>
+        <v>43376.5070486</v>
       </c>
       <c r="F26" s="3">
-        <v>43376.6320486</v>
+        <v>43376.5070486</v>
       </c>
       <c r="O26" s="0" t="s">
         <v>27</v>
@@ -1352,10 +1352,10 @@
         <v>2222244</v>
       </c>
       <c r="E27" s="2">
-        <v>43376.6480671</v>
+        <v>43376.5230671</v>
       </c>
       <c r="F27" s="3">
-        <v>43376.6480671</v>
+        <v>43376.5230671</v>
       </c>
       <c r="O27" s="0" t="s">
         <v>24</v>
@@ -1396,10 +1396,10 @@
         <v>123</v>
       </c>
       <c r="E28" s="2">
-        <v>43376.6488889</v>
+        <v>43376.5238889</v>
       </c>
       <c r="F28" s="3">
-        <v>43376.6488889</v>
+        <v>43376.5238889</v>
       </c>
       <c r="O28" s="0" t="s">
         <v>24</v>

</xml_diff>